<commit_message>
added live demo test case
</commit_message>
<xml_diff>
--- a/test/complex_test_case.xlsx
+++ b/test/complex_test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/forecasting-project/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED96B557-4AF1-2B4C-A6E6-5D85EF3F3769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76AF670-3816-A149-ADF1-AAC3CCC54D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="1520" windowWidth="20500" windowHeight="13600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13580" yWindow="1520" windowWidth="20500" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,10 +501,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>45658</v>
+        <v>46388</v>
       </c>
       <c r="D2" s="1">
-        <v>45838</v>
+        <v>46568</v>
       </c>
       <c r="E2">
         <v>5000</v>
@@ -518,10 +518,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1">
-        <v>45839</v>
+        <v>46569</v>
       </c>
       <c r="D3" s="1">
-        <v>46022</v>
+        <v>46752</v>
       </c>
       <c r="E3">
         <v>10000</v>
@@ -535,10 +535,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="1">
-        <v>45658</v>
+        <v>46388</v>
       </c>
       <c r="D4" s="1">
-        <v>46022</v>
+        <v>46752</v>
       </c>
       <c r="E4">
         <v>2000</v>
@@ -552,10 +552,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>45658</v>
+        <v>46388</v>
       </c>
       <c r="D5" s="1">
-        <v>46022</v>
+        <v>46752</v>
       </c>
       <c r="E5">
         <v>20000</v>
@@ -569,10 +569,10 @@
         <v>20</v>
       </c>
       <c r="C6" s="1">
-        <v>45658</v>
+        <v>46388</v>
       </c>
       <c r="D6" s="1">
-        <v>46022</v>
+        <v>46752</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>20100</v>
       </c>
       <c r="E2" s="3">
-        <v>45731</v>
+        <v>46461</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -649,7 +649,7 @@
         <v>4000</v>
       </c>
       <c r="E3" s="3">
-        <v>45703</v>
+        <v>46433</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -666,7 +666,7 @@
         <v>4000</v>
       </c>
       <c r="E4" s="3">
-        <v>45703</v>
+        <v>46433</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -683,7 +683,7 @@
         <v>2500</v>
       </c>
       <c r="E5" s="3">
-        <v>45762</v>
+        <v>46492</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -700,7 +700,7 @@
         <v>5000</v>
       </c>
       <c r="E6" s="3">
-        <v>45889</v>
+        <v>46619</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -717,7 +717,7 @@
         <v>1000</v>
       </c>
       <c r="E7" s="3">
-        <v>45823</v>
+        <v>46553</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>1000</v>
       </c>
       <c r="E8" s="3">
-        <v>46023</v>
+        <v>46753</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>500</v>
       </c>
       <c r="E9" s="3">
-        <v>45306</v>
+        <v>46037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>